<commit_message>
nombre de Hill non raréfié
</commit_message>
<xml_diff>
--- a/Output/tableau_abondance_par_site.xlsx
+++ b/Output/tableau_abondance_par_site.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,30 +365,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nombre d'individus observées</t>
+          <t>abon</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nombre d'espèces observées</t>
+          <t>N0</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>N0</t>
+          <t>N1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>N1</t>
+          <t>N2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>N2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
@@ -407,15 +402,12 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E2">
-        <v>19</v>
-      </c>
-      <c r="F2">
         <v>13</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Parc</t>
         </is>
@@ -434,15 +426,12 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -461,15 +450,12 @@
         <v>31</v>
       </c>
       <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
         <v>7</v>
       </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -488,15 +474,12 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5" t="inlineStr">
+        <v>17</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Parc</t>
         </is>
@@ -515,15 +498,12 @@
         <v>25</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -542,15 +522,12 @@
         <v>31</v>
       </c>
       <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
         <v>9</v>
       </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -569,15 +546,12 @@
         <v>41</v>
       </c>
       <c r="D8">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>13</v>
-      </c>
-      <c r="G8" t="inlineStr">
+        <v>21</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -596,15 +570,12 @@
         <v>36</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -617,21 +588,18 @@
         </is>
       </c>
       <c r="B10">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -650,15 +618,12 @@
         <v>38</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="G11" t="inlineStr">
+        <v>11</v>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -677,15 +642,12 @@
         <v>37</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>8</v>
-      </c>
-      <c r="G12" t="inlineStr">
+        <v>14</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -704,15 +666,12 @@
         <v>38</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>7</v>
-      </c>
-      <c r="G13" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>Parc</t>
         </is>
@@ -731,15 +690,12 @@
         <v>41</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E14">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
-      <c r="G14" t="inlineStr">
+        <v>13</v>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>Parc</t>
         </is>
@@ -758,15 +714,12 @@
         <v>39</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E15">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>9</v>
-      </c>
-      <c r="G15" t="inlineStr">
+        <v>15</v>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>Potager</t>
         </is>
@@ -785,15 +738,12 @@
         <v>44</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>6</v>
-      </c>
-      <c r="G16" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>Parc</t>
         </is>
@@ -806,7 +756,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>